<commit_message>
add charts and pdf
</commit_message>
<xml_diff>
--- a/uebung6/Messung.xlsx
+++ b/uebung6/Messung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -234,7 +234,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -462,11 +462,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8073615"/>
-        <c:axId val="71718064"/>
+        <c:axId val="82131980"/>
+        <c:axId val="85026077"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8073615"/>
+        <c:axId val="82131980"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,14 +522,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71718064"/>
+        <c:crossAx val="85026077"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71718064"/>
+        <c:axId val="85026077"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +594,825 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8073615"/>
+        <c:crossAx val="82131980"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:rPr>
+              <a:t>Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tx</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tx</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>UDP!$F$2:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TCP!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1036</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>358</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rx</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rx</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>UDP!$F$2:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TCP!$E$3:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>358</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="6039073"/>
+        <c:axId val="70273508"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="6039073"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70273508"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70273508"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6039073"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="DejaVu Sans"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:rPr>
+              <a:t>Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>tx</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tx</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>UDP!$B$2:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>UDP!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1370441</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2714828</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4068376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>rx</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rx</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>UDP!$B$2:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>UDP!$I$2:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1387755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2816568</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4080000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="87026523"/>
+        <c:axId val="92953787"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="87026523"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92953787"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92953787"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="DejaVu Sans"/>
+                  </a:rPr>
+                  <a:t>Bytes/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="DejaVu Sans"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87026523"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -677,9 +1495,74 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47160</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>183960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>175320</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>170640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1066680" y="1898280"/>
+        <a:ext cx="4207680" cy="2361600"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>153360</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546840</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Throughput"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5252400" y="1857600"/>
+        <a:ext cx="4216680" cy="2371680"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B1:M7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B1:M7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B1:M1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B1:M1"/>
   <tableColumns count="12">
     <tableColumn id="1" name="N"/>
     <tableColumn id="2" name="K"/>
@@ -1092,10 +1975,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,7 +1995,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +2033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="n">
         <v>10</v>
       </c>
@@ -1158,10 +2041,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1033</v>
+        <v>1042</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>997</v>
+        <v>1029</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1000</v>
@@ -1170,47 +2053,101 @@
         <v>1000</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1382381</v>
+        <v>1370441</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>1432296</v>
+        <v>1387755</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1355275</v>
+        <v>1343570</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1404212</v>
+        <v>1360544</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>1003</v>
+        <v>971</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>526</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>507</v>
+      </c>
       <c r="F3" s="0" t="n">
         <v>1000</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>2714828</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>2816568</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2661596</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>2761341</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1901</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>1972</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>350</v>
+      </c>
       <c r="F4" s="0" t="n">
         <v>1000</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>4068376</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>4080000</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>3988603</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2849</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>2857</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>10001</v>
       </c>
@@ -1218,396 +2155,201 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>524</v>
+        <v>79</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>675</v>
+        <v>91</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>5142</v>
+        <v>1000</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>27251908</v>
+        <v>18075949</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>15692307</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>26717557</v>
+        <v>17721518</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>15384615</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>19083</v>
+        <v>12658</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>10989</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
-        <v>10001</v>
+        <v>100001</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>615</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>775</v>
+      </c>
       <c r="F6" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>8365</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>23219512</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>15413187</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>22764227</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>15110967</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>16260</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>10793</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
-        <v>10001</v>
+        <v>1000001</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>6882</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>7046</v>
+      </c>
       <c r="F7" s="0" t="n">
-        <v>10000</v>
+        <v>100000</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>74888</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>20749782</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>15177414</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>20342923</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>14879818</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>14530</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>10628</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2031</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2008</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>703101</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>710444</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>689315</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>696513</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>492</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>497</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>13</v>
+      <c r="B9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>3031</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>471131</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>476000</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>461893</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>466666</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>333</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>1042</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>1029</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>971</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>1370441</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1387755</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>1343570</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>1360544</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>959</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>526</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>507</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>1972</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>2714828</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>2816568</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>2661596</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>2761341</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>1901</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>351</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>350</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>2857</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>4068376</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>4080000</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>3988603</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>2849</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>2857</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
-        <v>10001</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>91</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>10989</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>18075949</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>15692307</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>17721518</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>15384615</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>12658</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>10989</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
-        <v>10001</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>615</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>775</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>8365</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>10793</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>23219512</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>15413187</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>22764227</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>15110967</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <v>16260</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>10793</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
-        <v>10001</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>6882</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>7046</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>74888</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>10628</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>20749782</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>15177414</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>20342923</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>14879818</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <v>14530</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>10628</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>2031</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>2008</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>999</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>497</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>703101</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>710444</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>689315</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>696513</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>492</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>3031</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>333</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>471131</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>476000</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>461893</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>466666</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>329</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1616,8 +2358,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>